<commit_message>
make mds correctly negative
</commit_message>
<xml_diff>
--- a/docs/source/gbd2019_models/risk_risk_correlation/maternal_bmi_hgb_birthweight/md calculations.xlsx
+++ b/docs/source/gbd2019_models/risk_risk_correlation/maternal_bmi_hgb_birthweight/md calculations.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -447,16 +447,16 @@
         <v>1.962</v>
       </c>
       <c r="H2">
-        <f>D$5-D2</f>
-        <v>274.69999999999982</v>
+        <f>D2-D$5</f>
+        <v>-274.69999999999982</v>
       </c>
       <c r="I2">
         <f>$H2-$G2*$F2*SQRT(1/$C2+1/$C$5)</f>
-        <v>213.24048137102761</v>
+        <v>-336.15951862897202</v>
       </c>
       <c r="J2">
         <f>$H2+$G2*$F2*SQRT(1/$C2+1/$C$5)</f>
-        <v>336.15951862897202</v>
+        <v>-213.24048137102761</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
@@ -483,16 +483,16 @@
         <v>1.962</v>
       </c>
       <c r="H3">
-        <f>D$5-D3</f>
-        <v>181.90000000000009</v>
+        <f>D3-D$5</f>
+        <v>-181.90000000000009</v>
       </c>
       <c r="I3">
         <f>$H3-$G3*$F3*SQRT(1/$C3+1/$C$5)</f>
-        <v>42.44494319085041</v>
+        <v>-321.3550568091498</v>
       </c>
       <c r="J3">
         <f>$H3+$G3*$F3*SQRT(1/$C3+1/$C$5)</f>
-        <v>321.3550568091498</v>
+        <v>-42.44494319085041</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
@@ -519,16 +519,16 @@
         <v>1.962</v>
       </c>
       <c r="H4">
-        <f>D$5-D4</f>
-        <v>93.799999999999727</v>
+        <f>D4-D$5</f>
+        <v>-93.799999999999727</v>
       </c>
       <c r="I4">
         <f>$H4-$G4*$F4*SQRT(1/$C4+1/$C$5)</f>
-        <v>-3.662886302266017</v>
+        <v>-191.26288630226549</v>
       </c>
       <c r="J4">
         <f>$H4+$G4*$F4*SQRT(1/$C4+1/$C$5)</f>
-        <v>191.26288630226549</v>
+        <v>3.662886302266017</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
fixed error in pooled standard error calculation
</commit_message>
<xml_diff>
--- a/docs/source/gbd2019_models/risk_risk_correlation/maternal_bmi_hgb_birthweight/md calculations.xlsx
+++ b/docs/source/gbd2019_models/risk_risk_correlation/maternal_bmi_hgb_birthweight/md calculations.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -440,7 +440,7 @@
         <v>507.1</v>
       </c>
       <c r="F2">
-        <f>SQRT(((C2-1)*E2^2+(C$5-1)*E$5^2)/(C2+C5-2))</f>
+        <f>SQRT(((C2-1)*E2^2+(C$5-1)*E$5^2)/(C2+C$5-2))</f>
         <v>462.13648918971768</v>
       </c>
       <c r="G2">
@@ -476,8 +476,8 @@
         <v>460.7</v>
       </c>
       <c r="F3">
-        <f>SQRT(((C3-1)*E3^2+(C$5-1)*E$5^2)/(C3+C6-2))</f>
-        <v>1118.2714097652256</v>
+        <f>SQRT(((C3-1)*E3^2+(C$5-1)*E$5^2)/(C3+C$5-2))</f>
+        <v>455.12036591182641</v>
       </c>
       <c r="G3">
         <v>1.962</v>
@@ -488,11 +488,11 @@
       </c>
       <c r="I3">
         <f>$H3-$G3*$F3*SQRT(1/$C3+1/$C$5)</f>
-        <v>-321.3550568091498</v>
+        <v>-238.65620062267331</v>
       </c>
       <c r="J3">
         <f>$H3+$G3*$F3*SQRT(1/$C3+1/$C$5)</f>
-        <v>-42.44494319085041</v>
+        <v>-125.14379937732687</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.75">
@@ -512,8 +512,8 @@
         <v>515.1</v>
       </c>
       <c r="F4">
-        <f>SQRT(((C4-1)*E4^2+(C$5-1)*E$5^2)/(C4+C7-2))</f>
-        <v>949.15958549363017</v>
+        <f>SQRT(((C4-1)*E4^2+(C$5-1)*E$5^2)/(C4+C$5-2))</f>
+        <v>469.73206817174236</v>
       </c>
       <c r="G4">
         <v>1.962</v>
@@ -524,11 +524,11 @@
       </c>
       <c r="I4">
         <f>$H4-$G4*$F4*SQRT(1/$C4+1/$C$5)</f>
-        <v>-191.26288630226549</v>
+        <v>-142.03366254995024</v>
       </c>
       <c r="J4">
         <f>$H4+$G4*$F4*SQRT(1/$C4+1/$C$5)</f>
-        <v>3.662886302266017</v>
+        <v>-45.566337450049204</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">

</xml_diff>